<commit_message>
Created TournamentPlayer model and removed individual groups. Got loading tournament web scrape working for winnings.
</commit_message>
<xml_diff>
--- a/fg/external_files/the_open_groups.xlsx
+++ b/fg/external_files/the_open_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Library/Containers/com.microsoft.Excel/Data/Desktop/Projects/fgolf/fg/external_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EE08A6-6150-6547-961D-9DDA36DD9FF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C1507C-A255-6449-8050-5FAC44BBE0AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="460" windowWidth="23880" windowHeight="16420" xr2:uid="{C87BB418-C46E-474E-A92A-6B13B8DEC9CB}"/>
+    <workbookView xWindow="4920" yWindow="460" windowWidth="23880" windowHeight="16420" xr2:uid="{C87BB418-C46E-474E-A92A-6B13B8DEC9CB}"/>
   </bookViews>
   <sheets>
     <sheet name="the_open_groups" sheetId="1" r:id="rId1"/>
@@ -138,18 +138,9 @@
     <t>Adam Hadwin</t>
   </si>
   <si>
-    <t>Sungjae Im</t>
-  </si>
-  <si>
     <t>Sung Kang</t>
   </si>
   <si>
-    <t>Byeong Hun An</t>
-  </si>
-  <si>
-    <t>Rafa Cabrera Bello</t>
-  </si>
-  <si>
     <t>Tyrrell Hatton</t>
   </si>
   <si>
@@ -249,9 +240,6 @@
     <t>Darren Clarke</t>
   </si>
   <si>
-    <t>Ausin Connelly</t>
-  </si>
-  <si>
     <t>Corey Conners</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>Jazz Janewattananond</t>
   </si>
   <si>
-    <t>Dongkyu Jang</t>
-  </si>
-  <si>
     <t>Miguel Angel Jimenez</t>
   </si>
   <si>
@@ -306,21 +291,12 @@
     <t>Paul Waring</t>
   </si>
   <si>
-    <t>Brandon Wu</t>
-  </si>
-  <si>
     <t>Brian Harman</t>
   </si>
   <si>
-    <t>Innchoon Hwang</t>
-  </si>
-  <si>
     <t>Yuta Ikeda</t>
   </si>
   <si>
-    <t>Takumi Kanaya</t>
-  </si>
-  <si>
     <t>Chan Kim</t>
   </si>
   <si>
@@ -330,9 +306,6 @@
     <t>Patton Kizzire</t>
   </si>
   <si>
-    <t>Curtis Knipes</t>
-  </si>
-  <si>
     <t>Jason Kokrak</t>
   </si>
   <si>
@@ -357,9 +330,6 @@
     <t>Tom Lewis</t>
   </si>
   <si>
-    <t>Haotong Li</t>
-  </si>
-  <si>
     <t>David Lipsky</t>
   </si>
   <si>
@@ -372,9 +342,6 @@
     <t>Zander Lombard</t>
   </si>
   <si>
-    <t>Michael Lorenzo-Vera</t>
-  </si>
-  <si>
     <t>Joost Luiten</t>
   </si>
   <si>
@@ -393,9 +360,6 @@
     <t>Doyeob Mun</t>
   </si>
   <si>
-    <t>Alex Noren</t>
-  </si>
-  <si>
     <t>Shaun Norris</t>
   </si>
   <si>
@@ -408,12 +372,6 @@
     <t>C.T. Pan</t>
   </si>
   <si>
-    <t>Dimi Papadatos</t>
-  </si>
-  <si>
-    <t>Sanghyun Park</t>
-  </si>
-  <si>
     <t>Andrea Pavan</t>
   </si>
   <si>
@@ -435,9 +393,6 @@
     <t>Robert Rock</t>
   </si>
   <si>
-    <t>Matthias Schmid</t>
-  </si>
-  <si>
     <t>Jack Senior</t>
   </si>
   <si>
@@ -462,18 +417,12 @@
     <t>Kevin Streelman</t>
   </si>
   <si>
-    <t>James Sugrue</t>
-  </si>
-  <si>
     <t>Andy Sullivan</t>
   </si>
   <si>
     <t>Connor Syme</t>
   </si>
   <si>
-    <t>Thomas Thurloway</t>
-  </si>
-  <si>
     <t>Ashton Turner</t>
   </si>
   <si>
@@ -499,6 +448,57 @@
   </si>
   <si>
     <t>Ryan Palmer</t>
+  </si>
+  <si>
+    <t>Sung-jae Im</t>
+  </si>
+  <si>
+    <t>Byeong-Hun An</t>
+  </si>
+  <si>
+    <t>Rafael Cabrera Bello</t>
+  </si>
+  <si>
+    <t>Austin Connelly</t>
+  </si>
+  <si>
+    <t>Dong-Kyu Jang</t>
+  </si>
+  <si>
+    <t>Brandon Wu (a)</t>
+  </si>
+  <si>
+    <t>Inn-choon Hwang</t>
+  </si>
+  <si>
+    <t>Takumi Kanaya (a)</t>
+  </si>
+  <si>
+    <t>Curtis Knipes (a)</t>
+  </si>
+  <si>
+    <t>Li Haotong</t>
+  </si>
+  <si>
+    <t>Mike Lorenzo-Vera</t>
+  </si>
+  <si>
+    <t>Alexander Noren</t>
+  </si>
+  <si>
+    <t>Dimitrios Papadatos</t>
+  </si>
+  <si>
+    <t>Sang-hyun Park</t>
+  </si>
+  <si>
+    <t>Matthias Schmid (a)</t>
+  </si>
+  <si>
+    <t>James Sugrue (a)</t>
+  </si>
+  <si>
+    <t>Thomas Thurloway (a)</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,7 +883,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -911,7 +911,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -922,10 +922,10 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,10 +936,10 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -950,10 +950,10 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -964,10 +964,10 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -978,10 +978,10 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -992,10 +992,10 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1006,10 +1006,10 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,10 +1020,10 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1034,10 +1034,10 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1048,10 +1048,10 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1062,462 +1062,462 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D58" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D61" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D64" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D66" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D67" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D68" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D69" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D70" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D71" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D72" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D73" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D74" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D75" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D78" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>